<commit_message>
Adicionado arquivo Power BI
Arquivo em power bi possui comparação dos dois jogadores
</commit_message>
<xml_diff>
--- a/data/Nova pasta/titulosjuntos.xlsx
+++ b/data/Nova pasta/titulosjuntos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="102">
   <si>
     <t>Real Madrid CF</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Juventus FC</t>
-  </si>
-  <si>
-    <t>2X VENCEDOR DA SUPERTAÇA DA ITÁLIA</t>
   </si>
   <si>
     <t>Sporting CP</t>
@@ -332,9 +329,6 @@
   </si>
   <si>
     <t>FC Barcelona</t>
-  </si>
-  <si>
-    <t>10X CAMPEÃO DE ESPANHA</t>
   </si>
   <si>
     <t>21/22</t>
@@ -956,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -971,21 +965,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2">
         <v>2017</v>
@@ -994,12 +988,12 @@
         <v>0</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2">
         <v>2016</v>
@@ -1008,12 +1002,12 @@
         <v>0</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="2">
         <v>2008</v>
@@ -1022,82 +1016,82 @@
         <v>1</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B5" s="2">
         <v>2017</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B6" s="2">
         <v>2016</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2">
         <v>2014</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B8" s="2">
         <v>2013</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" s="2">
         <v>2008</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B10" s="2">
         <v>2017</v>
@@ -1106,12 +1100,12 @@
         <v>0</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B11" s="2">
         <v>2016</v>
@@ -1120,12 +1114,12 @@
         <v>0</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B12" s="2">
         <v>2014</v>
@@ -1134,12 +1128,12 @@
         <v>0</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B13" s="2">
         <v>2008</v>
@@ -1148,12 +1142,12 @@
         <v>1</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B14" s="2">
         <v>2018</v>
@@ -1162,12 +1156,12 @@
         <v>2</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2">
         <v>2017</v>
@@ -1176,12 +1170,12 @@
         <v>2</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" s="2">
         <v>2016</v>
@@ -1190,12 +1184,12 @@
         <v>2</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B17" s="2">
         <v>2015</v>
@@ -1204,12 +1198,12 @@
         <v>2</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2">
         <v>2013</v>
@@ -1218,12 +1212,12 @@
         <v>2</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B19" s="2">
         <v>2012</v>
@@ -1232,12 +1226,12 @@
         <v>2</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B20" s="2">
         <v>2011</v>
@@ -1246,12 +1240,12 @@
         <v>2</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B21" s="2">
         <v>2009</v>
@@ -1260,12 +1254,12 @@
         <v>2</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2">
         <v>2008</v>
@@ -1274,12 +1268,12 @@
         <v>2</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B23" s="2">
         <v>2007</v>
@@ -1288,54 +1282,54 @@
         <v>2</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1">
       <c r="A24" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30">
       <c r="A26" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
@@ -1344,222 +1338,222 @@
         <v>6</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="27">
       <c r="A37" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="42.75">
       <c r="A43" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B43" s="5">
         <v>2019</v>
@@ -1568,12 +1562,12 @@
         <v>12</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="42.75">
       <c r="A44" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B44" s="5">
         <v>2017</v>
@@ -1582,12 +1576,12 @@
         <v>13</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B45" s="5">
         <v>2016</v>
@@ -1596,12 +1590,12 @@
         <v>2</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>5</v>
@@ -1610,12 +1604,12 @@
         <v>0</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>7</v>
@@ -1624,12 +1618,12 @@
         <v>0</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>8</v>
@@ -1638,12 +1632,12 @@
         <v>0</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1">
       <c r="A49" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>10</v>
@@ -1652,26 +1646,26 @@
         <v>0</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1">
       <c r="A50" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1">
       <c r="A51" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B51" s="5">
         <v>2017</v>
@@ -1680,12 +1674,12 @@
         <v>0</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1">
       <c r="A52" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B52" s="5">
         <v>2016</v>
@@ -1694,12 +1688,12 @@
         <v>0</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1">
       <c r="A53" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B53" s="5">
         <v>2014</v>
@@ -1708,12 +1702,12 @@
         <v>0</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1">
       <c r="A54" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B54" s="5">
         <v>2008</v>
@@ -1722,12 +1716,12 @@
         <v>1</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1">
       <c r="A55" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B55" s="5">
         <v>2009</v>
@@ -1736,12 +1730,12 @@
         <v>1</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1">
       <c r="A56" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B56" s="5">
         <v>2008</v>
@@ -1750,12 +1744,12 @@
         <v>1</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1">
       <c r="A57" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B57" s="5">
         <v>2007</v>
@@ -1764,12 +1758,12 @@
         <v>1</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1">
       <c r="A58" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>7</v>
@@ -1778,12 +1772,12 @@
         <v>0</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1">
       <c r="A59" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B59" s="6">
         <v>45271</v>
@@ -1792,12 +1786,12 @@
         <v>0</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>14</v>
@@ -1806,12 +1800,12 @@
         <v>15</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>4</v>
@@ -1820,12 +1814,12 @@
         <v>15</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1">
       <c r="A62" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B62" s="5">
         <v>2019</v>
@@ -1834,12 +1828,12 @@
         <v>2</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1">
       <c r="A63" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>5</v>
@@ -1848,12 +1842,12 @@
         <v>0</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1">
       <c r="A64" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>7</v>
@@ -1862,12 +1856,12 @@
         <v>0</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1">
       <c r="A65" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>9</v>
@@ -1876,12 +1870,12 @@
         <v>0</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1">
       <c r="A66" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B66" s="5">
         <v>2004</v>
@@ -1890,12 +1884,12 @@
         <v>1</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1">
       <c r="A67" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>10</v>
@@ -1904,26 +1898,26 @@
         <v>0</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1">
       <c r="A68" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1">
       <c r="A69" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>3</v>
@@ -1932,12 +1926,12 @@
         <v>15</v>
       </c>
       <c r="D69" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="28.5">
       <c r="A70" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B70" s="5">
         <v>2009</v>
@@ -1946,12 +1940,12 @@
         <v>1</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="28.5">
       <c r="A71" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B71" s="5">
         <v>2006</v>
@@ -1960,12 +1954,12 @@
         <v>1</v>
       </c>
       <c r="D71" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="28.5">
       <c r="A72" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>5</v>
@@ -1974,26 +1968,26 @@
         <v>0</v>
       </c>
       <c r="D72" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="28.5">
       <c r="A73" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D73" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>3</v>
@@ -2002,12 +1996,12 @@
         <v>15</v>
       </c>
       <c r="D74" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1">
       <c r="A75" s="11" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>4</v>
@@ -2016,12 +2010,12 @@
         <v>15</v>
       </c>
       <c r="D75" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="28.5">
       <c r="A76" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B76" s="5">
         <v>2008</v>
@@ -2030,12 +2024,12 @@
         <v>1</v>
       </c>
       <c r="D76" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="28.5">
       <c r="A77" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B77" s="5">
         <v>2007</v>
@@ -2044,516 +2038,516 @@
         <v>1</v>
       </c>
       <c r="D77" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="28.5">
       <c r="A78" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B78" s="5">
         <v>2002</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B79" s="14">
         <v>2022</v>
       </c>
       <c r="C79" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D79" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B80" s="14">
         <v>2019</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D80" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B81" s="14">
         <v>2009</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D81" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B82" s="14">
         <v>2021</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D82" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B83" s="14">
         <v>2019</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D83" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B84" s="14">
         <v>2015</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B85" s="14">
         <v>2012</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B86" s="14">
         <v>2011</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B87" s="14">
         <v>2010</v>
       </c>
       <c r="C87" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D87" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B88" s="14">
         <v>2009</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D88" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B89" s="14">
         <v>2015</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D89" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B90" s="14">
         <v>2011</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D90" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B91" s="14">
         <v>2009</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D91" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B92" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C92" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D92" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B93" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C93" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D93" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B94" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C94" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D94" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B95" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C95" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D95" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B96" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C96" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D96" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B97" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C97" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D97" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B98" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D98" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B99" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C99" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D99" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B100" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C100" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D100" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B101" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C101" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D101" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B102" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C102" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D102" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C103" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D103" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C104" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D104" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C105" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D105" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C106" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D106" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C107" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D107" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C108" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D108" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C109" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D109" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D110" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C111" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D111" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C112" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D112" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="24">
       <c r="A113" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D113" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="42.75">
       <c r="A114" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B114" s="14">
         <v>2021</v>
@@ -2562,12 +2556,12 @@
         <v>13</v>
       </c>
       <c r="D114" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="42.75">
       <c r="A115" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B115" s="14">
         <v>2020</v>
@@ -2576,12 +2570,12 @@
         <v>13</v>
       </c>
       <c r="D115" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="42.75">
       <c r="A116" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B116" s="14">
         <v>2019</v>
@@ -2590,12 +2584,12 @@
         <v>13</v>
       </c>
       <c r="D116" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="42.75">
       <c r="A117" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B117" s="14">
         <v>2018</v>
@@ -2604,595 +2598,595 @@
         <v>13</v>
       </c>
       <c r="D117" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B118" s="16">
         <v>2022</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D118" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B119" s="16" t="s">
         <v>3</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D119" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B120" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D120" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B121" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D121" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D122" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D123" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B124" s="16">
         <v>2016</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D124" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B125" s="16">
         <v>2012</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D125" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B126" s="16">
         <v>2010</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D126" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B127" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D127" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="13" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B128" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D128" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="13" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B129" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D129" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="13" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B130" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D130" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="13" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D131" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="13" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B132" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D132" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="13" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B133" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D133" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="13" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B134" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D134" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="13" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B135" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D135" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="13" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B136" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D136" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D137" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B138" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D138" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B139" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D139" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B140" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D140" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B141" s="16" t="s">
         <v>3</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D141" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B142" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D142" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B143" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D143" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B144" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D144" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B145" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D145" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B146" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D146" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B147" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D147" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="28.5">
       <c r="A148" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B148" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D148" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="28.5">
       <c r="A149" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B149" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D149" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="28.5">
       <c r="A150" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B150" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D150" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="28.5">
       <c r="A151" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B151" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D151" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="28.5">
       <c r="A152" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B152" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D152" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="28.5">
       <c r="A153" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B153" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D153" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="28.5">
       <c r="A154" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B154" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D154" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="28.5">
       <c r="A155" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B155" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D155" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B156" s="17">
         <v>2005</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D156" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="28.5">
       <c r="A157" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B157" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D157" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B158" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D158" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B159" s="18">
         <v>45177</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D159" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>